<commit_message>
new versions of excel files
</commit_message>
<xml_diff>
--- a/docs/unit1/03_darcy_layered/layers.xlsx
+++ b/docs/unit1/03_darcy_layered/layers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/My Drive (njones61@gmail.com)/work - byu/courses/CE 544/exercises/3. darcy's law - layered systems, 2d/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/My Drive (njones61@gmail.com)/work - byu/courses/CE 544/exercises/3. darcy's law, layered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B24B555-DCB0-8948-AD10-E037118E658C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9722B7-0BCD-F449-A695-29FAF05CB88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16040" yWindow="3540" windowWidth="26840" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23240" yWindow="4300" windowWidth="30880" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+  <numFmts count="5">
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="172" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -251,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,47 +278,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,6 +409,159 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CAABD66-D11A-70C4-8B32-85B49AEE6F5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6591300" y="3263900"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>296334</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>23281</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C5741A6-6BCA-4338-ABA0-F88C0C4A3B21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6593417" y="645584"/>
+          <a:ext cx="5725584" cy="2256364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>40217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{464FAA7A-17BC-DD2A-ADB1-F42B03564BF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6466417" y="3471334"/>
+          <a:ext cx="5905500" cy="1765300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -684,7 +855,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -748,25 +919,25 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -777,16 +948,16 @@
       <c r="B11" s="4">
         <v>1E-3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="15">
         <f>B11/(12*2.54)*(3600*24)</f>
         <v>2.8346456692913384</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -796,16 +967,16 @@
         <f>10^(-7)</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="16">
         <f>B12/(12*2.54)*(3600*24)</f>
         <v>2.8346456692913383E-4</v>
       </c>
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -814,16 +985,16 @@
       <c r="B13" s="4">
         <v>0.1</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="17">
         <f>B13/(12*2.54)*(3600*24)</f>
         <v>283.46456692913387</v>
       </c>
       <c r="D13" s="3">
         <v>8</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="17"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
@@ -832,27 +1003,30 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="19">
+        <f>SUM(G11:G13)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="24"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="19"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="10" t="s">
         <v>12</v>
       </c>
@@ -863,25 +1037,25 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -892,16 +1066,16 @@
       <c r="B23" s="4">
         <v>1E-3</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="15">
         <f>B23/(12*2.54)*(3600*24)</f>
         <v>2.8346456692913384</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
@@ -911,16 +1085,16 @@
         <f>10^(-7)</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="16">
         <f>B24/(12*2.54)*(3600*24)</f>
         <v>2.8346456692913383E-4</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -929,16 +1103,16 @@
       <c r="B25" s="4">
         <v>0.1</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="17">
         <f>B25/(12*2.54)*(3600*24)</f>
         <v>283.46456692913387</v>
       </c>
       <c r="D25" s="3">
         <v>8</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="12"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
@@ -946,30 +1120,33 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="20"/>
+      <c r="F26" s="12">
+        <f>SUM(F23:F25)</f>
+        <v>0</v>
+      </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="24"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="8"/>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>